<commit_message>
Last minute changes in PP to prevent all unforeseen collisions
</commit_message>
<xml_diff>
--- a/test/sum-of-costs.xlsx
+++ b/test/sum-of-costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobharrington/Public/CSCI-360/Project_3/code/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E33934F-F982-7744-BCBB-D24086D279F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D53CC6-279B-464A-9951-EA356159D1AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{4A33544D-D16C-459C-8927-8DE463C63322}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4A33544D-D16C-459C-8927-8DE463C63322}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="9">
   <si>
     <t>CBS</t>
   </si>
@@ -47,12 +47,18 @@
   <si>
     <t>Results: Sum of costs</t>
   </si>
+  <si>
+    <t xml:space="preserve"> (Note1)</t>
+  </si>
+  <si>
+    <t>Note 1: As announced, Prioritized Planning  is suboptimal and may fluctuate in solutions; thereby, this metric need not be met so long as no collisions occur and agents obey hierarchy.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,19 +72,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -94,13 +101,8 @@
         <bgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="gray0625">
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -142,10 +144,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -265,90 +276,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -665,237 +703,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB35C2D-5E06-480A-8A54-37B121077658}">
-  <dimension ref="A1:XFB52"/>
+  <dimension ref="A1:XFB56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5 16382:16382" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="12"/>
+      <c r="E1" s="13"/>
       <c r="XFB1" s="2"/>
     </row>
     <row r="2" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="26" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="24" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A3" s="15">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
       <c r="B3" s="19">
         <v>41</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="7">
         <v>49</v>
       </c>
-      <c r="D3" s="23">
-        <v>50</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>3</v>
+      <c r="D3" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="26">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A4" s="14">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
       <c r="B4" s="20">
         <v>18</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>18</v>
       </c>
-      <c r="D4" s="24">
-        <v>18</v>
+      <c r="D4" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E4" s="4">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A5" s="14">
+      <c r="A5" s="15">
         <v>3</v>
       </c>
       <c r="B5" s="20">
         <v>28</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>28</v>
       </c>
-      <c r="D5" s="24">
-        <v>28</v>
+      <c r="D5" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E5" s="4">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A6" s="14">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
       <c r="B6" s="20">
         <v>32</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>33</v>
       </c>
-      <c r="D6" s="24">
-        <v>32</v>
+      <c r="D6" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E6" s="4">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A7" s="14">
+      <c r="A7" s="15">
         <v>5</v>
       </c>
       <c r="B7" s="20">
         <v>26</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>27</v>
       </c>
-      <c r="D7" s="24">
-        <v>27</v>
+      <c r="D7" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E7" s="4">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A8" s="14">
+      <c r="A8" s="15">
         <v>6</v>
       </c>
       <c r="B8" s="20">
         <v>24</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>26</v>
       </c>
-      <c r="D8" s="24">
-        <v>25</v>
+      <c r="D8" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E8" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A9" s="14">
+      <c r="A9" s="15">
         <v>7</v>
       </c>
       <c r="B9" s="20">
         <v>34</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>35</v>
       </c>
-      <c r="D9" s="24">
-        <v>35</v>
+      <c r="D9" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E9" s="4">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A10" s="14">
+      <c r="A10" s="15">
         <v>8</v>
       </c>
       <c r="B10" s="20">
         <v>38</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <v>44</v>
       </c>
-      <c r="D10" s="24">
-        <v>42</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A11" s="14">
+      <c r="A11" s="15">
         <v>9</v>
       </c>
       <c r="B11" s="20">
         <v>24</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <v>24</v>
       </c>
-      <c r="D11" s="24">
-        <v>24</v>
+      <c r="D11" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E11" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A12" s="14">
+      <c r="A12" s="15">
         <v>10</v>
       </c>
       <c r="B12" s="20">
         <v>19</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <v>23</v>
       </c>
-      <c r="D12" s="24">
-        <v>20</v>
+      <c r="D12" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E12" s="4">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A13" s="14">
+      <c r="A13" s="15">
         <v>11</v>
       </c>
       <c r="B13" s="20">
         <v>35</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="5">
         <v>35</v>
       </c>
-      <c r="D13" s="24">
-        <v>35</v>
+      <c r="D13" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E13" s="4">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A14" s="14">
+      <c r="A14" s="15">
         <v>12</v>
       </c>
       <c r="B14" s="20">
@@ -904,49 +942,49 @@
       <c r="C14" s="7">
         <v>38</v>
       </c>
-      <c r="D14" s="20">
-        <v>36</v>
+      <c r="D14" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E14" s="4">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A15" s="14">
+      <c r="A15" s="15">
         <v>13</v>
       </c>
       <c r="B15" s="20">
         <v>36</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="5">
         <v>45</v>
       </c>
-      <c r="D15" s="24">
-        <v>45</v>
+      <c r="D15" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E15" s="4">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5 16382:16382" x14ac:dyDescent="0.2">
-      <c r="A16" s="14">
+      <c r="A16" s="15">
         <v>14</v>
       </c>
       <c r="B16" s="20">
         <v>24</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="5">
         <v>24</v>
       </c>
-      <c r="D16" s="24">
-        <v>24</v>
+      <c r="D16" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E16" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16">
+      <c r="A17" s="17">
         <v>15</v>
       </c>
       <c r="B17" s="21">
@@ -955,15 +993,15 @@
       <c r="C17" s="8">
         <v>52</v>
       </c>
-      <c r="D17" s="21">
-        <v>52</v>
+      <c r="D17" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E17" s="4">
         <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="15">
+      <c r="A18" s="16">
         <v>16</v>
       </c>
       <c r="B18" s="19">
@@ -972,117 +1010,117 @@
       <c r="C18" s="7">
         <v>53</v>
       </c>
-      <c r="D18" s="24">
-        <v>53</v>
+      <c r="D18" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="14">
+      <c r="A19" s="15">
         <v>17</v>
       </c>
       <c r="B19" s="20">
         <v>39</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="5">
         <v>41</v>
       </c>
-      <c r="D19" s="24">
-        <v>40</v>
+      <c r="D19" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E19" s="4">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="14">
+      <c r="A20" s="15">
         <v>18</v>
       </c>
       <c r="B20" s="20">
         <v>32</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="5">
         <v>32</v>
       </c>
-      <c r="D20" s="24">
-        <v>32</v>
+      <c r="D20" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E20" s="4">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="14">
+      <c r="A21" s="15">
         <v>19</v>
       </c>
       <c r="B21" s="20">
         <v>47</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="5">
         <v>49</v>
       </c>
-      <c r="D21" s="24">
-        <v>49</v>
+      <c r="D21" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E21" s="4">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="14">
+      <c r="A22" s="15">
         <v>20</v>
       </c>
       <c r="B22" s="20">
         <v>28</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="5">
         <v>33</v>
       </c>
-      <c r="D22" s="24">
-        <v>29</v>
+      <c r="D22" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E22" s="4">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="14">
+      <c r="A23" s="15">
         <v>21</v>
       </c>
       <c r="B23" s="20">
         <v>46</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="5">
         <v>47</v>
       </c>
-      <c r="D23" s="24">
-        <v>47</v>
+      <c r="D23" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E23" s="4">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="14">
+      <c r="A24" s="15">
         <v>22</v>
       </c>
       <c r="B24" s="20">
         <v>51</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="5">
         <v>54</v>
       </c>
-      <c r="D24" s="24">
-        <v>52</v>
+      <c r="D24" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E24" s="4">
         <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="14">
+      <c r="A25" s="15">
         <v>23</v>
       </c>
       <c r="B25" s="20">
@@ -1091,25 +1129,25 @@
       <c r="C25" s="7">
         <v>32</v>
       </c>
-      <c r="D25" s="20">
-        <v>32</v>
+      <c r="D25" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E25" s="4">
         <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="15">
+      <c r="A26" s="16">
         <v>24</v>
       </c>
       <c r="B26" s="19">
         <v>47</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="5">
         <v>48</v>
       </c>
-      <c r="D26" s="24">
-        <v>46</v>
+      <c r="D26" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>3</v>
@@ -1125,49 +1163,49 @@
       <c r="C27" s="7">
         <v>-1</v>
       </c>
-      <c r="D27" s="20">
-        <v>-1</v>
+      <c r="D27" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E27" s="4">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="14">
+      <c r="A28" s="15">
         <v>26</v>
       </c>
       <c r="B28" s="20">
         <v>42</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="5">
         <v>42</v>
       </c>
-      <c r="D28" s="24">
-        <v>42</v>
+      <c r="D28" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E28" s="4">
         <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="14">
+      <c r="A29" s="15">
         <v>27</v>
       </c>
       <c r="B29" s="20">
         <v>40</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="5">
         <v>47</v>
       </c>
-      <c r="D29" s="24">
-        <v>45</v>
+      <c r="D29" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E29" s="4">
         <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="14">
+      <c r="A30" s="15">
         <v>28</v>
       </c>
       <c r="B30" s="20">
@@ -1176,117 +1214,117 @@
       <c r="C30" s="7">
         <v>41</v>
       </c>
-      <c r="D30" s="20">
-        <v>42</v>
+      <c r="D30" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E30" s="4">
         <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="14">
+      <c r="A31" s="15">
         <v>29</v>
       </c>
       <c r="B31" s="20">
         <v>48</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="5">
         <v>52</v>
       </c>
-      <c r="D31" s="24">
-        <v>51</v>
+      <c r="D31" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E31" s="4">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="15">
+      <c r="A32" s="16">
         <v>30</v>
       </c>
       <c r="B32" s="19">
         <v>43</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="5">
         <v>49</v>
       </c>
-      <c r="D32" s="24">
-        <v>43</v>
+      <c r="D32" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="17">
+      <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="B33" s="20">
         <v>39</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="7">
         <v>39</v>
       </c>
-      <c r="D33" s="23">
-        <v>37</v>
+      <c r="D33" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E33" s="4">
         <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="14">
+      <c r="A34" s="15">
         <v>32</v>
       </c>
       <c r="B34" s="20">
         <v>30</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="5">
         <v>30</v>
       </c>
-      <c r="D34" s="24">
-        <v>30</v>
+      <c r="D34" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E34" s="4">
         <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="15">
+      <c r="A35" s="16">
         <v>33</v>
       </c>
       <c r="B35" s="19">
         <v>28</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="5">
         <v>31</v>
       </c>
-      <c r="D35" s="24">
-        <v>31</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>3</v>
+      <c r="D35" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="14">
+      <c r="A36" s="15">
         <v>34</v>
       </c>
       <c r="B36" s="20">
         <v>33</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="5">
         <v>34</v>
       </c>
-      <c r="D36" s="24">
-        <v>34</v>
+      <c r="D36" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E36" s="4">
         <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="14">
+      <c r="A37" s="15">
         <v>35</v>
       </c>
       <c r="B37" s="20">
@@ -1295,151 +1333,151 @@
       <c r="C37" s="7">
         <v>32</v>
       </c>
-      <c r="D37" s="20">
-        <v>32</v>
+      <c r="D37" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E37" s="4">
         <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="14">
+      <c r="A38" s="15">
         <v>36</v>
       </c>
       <c r="B38" s="20">
         <v>23</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="5">
         <v>23</v>
       </c>
-      <c r="D38" s="24">
-        <v>23</v>
+      <c r="D38" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E38" s="4">
         <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="14">
+      <c r="A39" s="15">
         <v>37</v>
       </c>
       <c r="B39" s="20">
         <v>38</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="5">
         <v>38</v>
       </c>
-      <c r="D39" s="24">
-        <v>38</v>
+      <c r="D39" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E39" s="4">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="14">
+      <c r="A40" s="15">
         <v>38</v>
       </c>
       <c r="B40" s="20">
         <v>28</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="5">
         <v>28</v>
       </c>
-      <c r="D40" s="24">
-        <v>28</v>
+      <c r="D40" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E40" s="4">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="14">
+      <c r="A41" s="15">
         <v>39</v>
       </c>
       <c r="B41" s="20">
         <v>35</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="5">
         <v>39</v>
       </c>
-      <c r="D41" s="24">
-        <v>35</v>
+      <c r="D41" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E41" s="4">
         <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="14">
+      <c r="A42" s="15">
         <v>40</v>
       </c>
       <c r="B42" s="20">
         <v>24</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="5">
         <v>24</v>
       </c>
-      <c r="D42" s="24">
-        <v>24</v>
+      <c r="D42" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E42" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="15">
+      <c r="A43" s="16">
         <v>41</v>
       </c>
       <c r="B43" s="19">
         <v>45</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="5">
         <v>45</v>
       </c>
-      <c r="D43" s="24">
-        <v>45</v>
+      <c r="D43" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="15">
+      <c r="A44" s="16">
         <v>42</v>
       </c>
       <c r="B44" s="19">
         <v>57</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="5">
         <v>63</v>
       </c>
-      <c r="D44" s="24">
-        <v>56</v>
+      <c r="D44" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="14">
+      <c r="A45" s="15">
         <v>43</v>
       </c>
       <c r="B45" s="20">
         <v>43</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="5">
         <v>48</v>
       </c>
-      <c r="D45" s="24">
-        <v>46</v>
+      <c r="D45" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E45" s="4">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="14">
+      <c r="A46" s="15">
         <v>44</v>
       </c>
       <c r="B46" s="20">
@@ -1448,15 +1486,15 @@
       <c r="C46" s="7">
         <v>36</v>
       </c>
-      <c r="D46" s="20">
-        <v>34</v>
+      <c r="D46" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E46" s="4">
         <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="14">
+      <c r="A47" s="15">
         <v>45</v>
       </c>
       <c r="B47" s="20">
@@ -1465,15 +1503,15 @@
       <c r="C47" s="7">
         <v>24</v>
       </c>
-      <c r="D47" s="20">
-        <v>24</v>
+      <c r="D47" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E47" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="14">
+      <c r="A48" s="15">
         <v>46</v>
       </c>
       <c r="B48" s="20">
@@ -1482,15 +1520,15 @@
       <c r="C48" s="7">
         <v>59</v>
       </c>
-      <c r="D48" s="20">
-        <v>59</v>
+      <c r="D48" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E48" s="4">
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="15">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="16">
         <v>47</v>
       </c>
       <c r="B49" s="19">
@@ -1499,15 +1537,15 @@
       <c r="C49" s="7">
         <v>75</v>
       </c>
-      <c r="D49" s="20">
-        <v>68</v>
+      <c r="D49" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="14">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="15">
         <v>48</v>
       </c>
       <c r="B50" s="20">
@@ -1516,51 +1554,89 @@
       <c r="C50" s="7">
         <v>38</v>
       </c>
-      <c r="D50" s="24">
-        <v>36</v>
+      <c r="D50" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E50" s="4">
         <v>36</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="14">
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="15">
         <v>49</v>
       </c>
       <c r="B51" s="20">
         <v>42</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="5">
         <v>44</v>
       </c>
-      <c r="D51" s="24">
-        <v>42</v>
+      <c r="D51" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E51" s="4">
         <v>42</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18">
         <v>50</v>
       </c>
       <c r="B52" s="22">
         <v>48</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C52" s="10">
         <v>58</v>
       </c>
-      <c r="D52" s="25">
-        <v>58</v>
-      </c>
-      <c r="E52" s="9">
-        <v>50</v>
-      </c>
+      <c r="D52" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="29">
+        <v>48</v>
+      </c>
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="27"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="27"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A53:F56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>